<commit_message>
add fpga ipc test
</commit_message>
<xml_diff>
--- a/开题/测试/IPC性能.xlsx
+++ b/开题/测试/IPC性能.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ctrlz/workSpace/openingreport-ldhai2023/开题/测试/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA131BF-7343-2348-9F4C-DDB1E98D7376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEBA1BE9-3730-3E4E-BED8-7325384A53FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16680" activeTab="2" xr2:uid="{DA4805F4-04B1-CA43-9DDD-E0DA8EA5F629}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="43">
   <si>
     <t>async-smp</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,12 +161,59 @@
     <t>负载3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Server Phase</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLI Phase 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CLI Phase 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fetch task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fill &amp; send msg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get req</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>write reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get reply</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wake task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>sync-up-fp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -179,6 +226,31 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -205,9 +277,24 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1595,8 +1682,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1858,7 +1946,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>qemu_ipc!$M$3</c:f>
+              <c:f>qemu_ipc!$AM$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1907,7 +1995,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$2:$S$2</c:f>
+              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1934,7 +2022,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$3:$S$3</c:f>
+              <c:f>qemu_ipc!$AN$16:$AS$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1971,7 +2059,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>qemu_ipc!$M$4</c:f>
+              <c:f>qemu_ipc!$AM$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2020,7 +2108,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$2:$S$2</c:f>
+              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2047,7 +2135,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$4:$S$4</c:f>
+              <c:f>qemu_ipc!$AN$17:$AS$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2084,7 +2172,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>qemu_ipc!$M$5</c:f>
+              <c:f>qemu_ipc!$AM$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2133,7 +2221,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$2:$S$2</c:f>
+              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2160,7 +2248,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$5:$S$5</c:f>
+              <c:f>qemu_ipc!$AN$18:$AS$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2197,7 +2285,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>qemu_ipc!$M$6</c:f>
+              <c:f>qemu_ipc!$AM$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2246,7 +2334,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$2:$S$2</c:f>
+              <c:f>qemu_ipc!$AN$15:$AS$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2273,7 +2361,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$6:$S$6</c:f>
+              <c:f>qemu_ipc!$AN$19:$AS$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -2598,7 +2686,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>qemu_ipc!$M$26</c:f>
+              <c:f>qemu_ipc!$AM$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2647,7 +2735,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>qemu_ipc!$N$25:$Q$25</c:f>
+              <c:f>qemu_ipc!$AN$38:$AQ$38</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2667,7 +2755,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$26:$Q$26</c:f>
+              <c:f>qemu_ipc!$AN$39:$AQ$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2698,7 +2786,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>qemu_ipc!$M$27</c:f>
+              <c:f>qemu_ipc!$AM$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2747,7 +2835,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>qemu_ipc!$N$25:$Q$25</c:f>
+              <c:f>qemu_ipc!$AN$38:$AQ$38</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2767,7 +2855,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$27:$Q$27</c:f>
+              <c:f>qemu_ipc!$AN$40:$AQ$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2798,7 +2886,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>qemu_ipc!$M$28</c:f>
+              <c:f>qemu_ipc!$AM$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2847,7 +2935,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>qemu_ipc!$N$25:$Q$25</c:f>
+              <c:f>qemu_ipc!$AN$38:$AQ$38</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2867,7 +2955,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$28:$Q$28</c:f>
+              <c:f>qemu_ipc!$AN$41:$AQ$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2898,7 +2986,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>qemu_ipc!$M$29</c:f>
+              <c:f>qemu_ipc!$AM$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2947,7 +3035,7 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>qemu_ipc!$N$25:$Q$25</c:f>
+              <c:f>qemu_ipc!$AN$38:$AQ$38</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -2967,7 +3055,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>qemu_ipc!$N$29:$Q$29</c:f>
+              <c:f>qemu_ipc!$AN$42:$AQ$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -6198,35 +6286,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -6287,10 +6346,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>fpga_ipc!$B$3:$G$3</c:f>
+              <c:f>fpga_ipc!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6308,33 +6367,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>fpga_ipc!$B$4:$G$4</c:f>
+              <c:f>fpga_ipc!$B$4:$H$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>8920</c:v>
+                  <c:v>6648</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6004</c:v>
+                  <c:v>3908</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4458</c:v>
+                  <c:v>2437</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3746</c:v>
+                  <c:v>1766</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3332</c:v>
+                  <c:v>1547</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3111</c:v>
+                  <c:v>1421</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1358</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6342,7 +6407,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-FB7D-C746-88E0-D8950AEBE751}"/>
+              <c16:uniqueId val="{00000002-ECC1-4347-AF1B-106F62193857}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6400,10 +6465,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>fpga_ipc!$B$3:$G$3</c:f>
+              <c:f>fpga_ipc!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6421,33 +6486,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>fpga_ipc!$B$5:$G$5</c:f>
+              <c:f>fpga_ipc!$B$5:$H$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>7419</c:v>
+                  <c:v>6327</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5618</c:v>
+                  <c:v>3649</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4219</c:v>
+                  <c:v>2187</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3639</c:v>
+                  <c:v>1799</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3198</c:v>
+                  <c:v>1643</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3008</c:v>
+                  <c:v>1504</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1517</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6455,7 +6526,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-FB7D-C746-88E0-D8950AEBE751}"/>
+              <c16:uniqueId val="{00000003-ECC1-4347-AF1B-106F62193857}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6513,10 +6584,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>fpga_ipc!$B$3:$G$3</c:f>
+              <c:f>fpga_ipc!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6534,33 +6605,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>fpga_ipc!$B$6:$G$6</c:f>
+              <c:f>fpga_ipc!$B$6:$H$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2141</c:v>
+                  <c:v>2868</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2141</c:v>
+                  <c:v>2868</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2141</c:v>
+                  <c:v>2868</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2141</c:v>
+                  <c:v>2868</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2141</c:v>
+                  <c:v>2868</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2141</c:v>
+                  <c:v>2868</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6568,7 +6645,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FB7D-C746-88E0-D8950AEBE751}"/>
+              <c16:uniqueId val="{00000004-ECC1-4347-AF1B-106F62193857}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6581,7 +6658,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>sync-smp</c:v>
+                  <c:v>sync-up-fp</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6626,10 +6703,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>fpga_ipc!$B$3:$G$3</c:f>
+              <c:f>fpga_ipc!$B$3:$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6647,33 +6724,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>fpga_ipc!$B$7:$G$7</c:f>
+              <c:f>fpga_ipc!$B$7:$H$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6283</c:v>
+                  <c:v>2141</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6283</c:v>
+                  <c:v>2141</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6283</c:v>
+                  <c:v>2141</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6283</c:v>
+                  <c:v>2141</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6283</c:v>
+                  <c:v>2141</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6283</c:v>
+                  <c:v>2141</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2141</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6681,7 +6764,126 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-FB7D-C746-88E0-D8950AEBE751}"/>
+              <c16:uniqueId val="{00000005-ECC1-4347-AF1B-106F62193857}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>fpga_ipc!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sync-smp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>fpga_ipc!$B$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>fpga_ipc!$B$8:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6283</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6283</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6283</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6283</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6283</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6283</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6283</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-ECC1-4347-AF1B-106F62193857}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -7412,8 +7614,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -13373,15 +13576,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>645305</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>124112</xdr:rowOff>
+      <xdr:colOff>670705</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>187612</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>117231</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>146538</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13408,15 +13611,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>45</xdr:col>
       <xdr:colOff>465209</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>165552</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
+      <xdr:col>55</xdr:col>
       <xdr:colOff>258773</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>126774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13444,15 +13647,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>792393</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>32565</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>44</xdr:col>
       <xdr:colOff>109632</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>58182</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14040,10 +14243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EE31C07-FDF3-8D4E-AAE0-9812488F355C}">
-  <dimension ref="A1:AA29"/>
+  <dimension ref="A2:BA42"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25:Q29"/>
+    <sheetView zoomScale="131" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AP12" sqref="AP12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14052,15 +14255,7 @@
     <col min="13" max="13" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
-      <c r="M1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:53">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -14088,50 +14283,8 @@
       <c r="I2">
         <v>128</v>
       </c>
-      <c r="M2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>2</v>
-      </c>
-      <c r="P2">
-        <v>4</v>
-      </c>
-      <c r="Q2">
-        <v>8</v>
-      </c>
-      <c r="R2">
-        <v>16</v>
-      </c>
-      <c r="S2">
-        <v>32</v>
-      </c>
-      <c r="U2" t="s">
-        <v>14</v>
-      </c>
-      <c r="V2">
-        <v>1</v>
-      </c>
-      <c r="W2">
-        <v>2</v>
-      </c>
-      <c r="X2">
-        <v>4</v>
-      </c>
-      <c r="Y2">
-        <v>8</v>
-      </c>
-      <c r="Z2">
-        <v>16</v>
-      </c>
-      <c r="AA2">
-        <v>32</v>
-      </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:53">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -14159,577 +14312,637 @@
       <c r="I3">
         <v>251</v>
       </c>
-      <c r="M3" t="s">
+    </row>
+    <row r="4" spans="1:53">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1248</v>
+      </c>
+      <c r="C4">
+        <v>642</v>
+      </c>
+      <c r="D4">
+        <v>434</v>
+      </c>
+      <c r="E4">
+        <v>344</v>
+      </c>
+      <c r="F4">
+        <v>315</v>
+      </c>
+      <c r="G4">
+        <v>307</v>
+      </c>
+      <c r="H4">
+        <v>298</v>
+      </c>
+      <c r="I4">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:53">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>535</v>
+      </c>
+      <c r="C5">
+        <v>535</v>
+      </c>
+      <c r="D5">
+        <v>535</v>
+      </c>
+      <c r="E5">
+        <v>535</v>
+      </c>
+      <c r="F5">
+        <v>535</v>
+      </c>
+      <c r="G5">
+        <v>535</v>
+      </c>
+      <c r="H5">
+        <v>535</v>
+      </c>
+      <c r="I5">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="6" spans="1:53">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1813</v>
+      </c>
+      <c r="C6">
+        <v>1813</v>
+      </c>
+      <c r="D6">
+        <v>1813</v>
+      </c>
+      <c r="E6">
+        <v>1813</v>
+      </c>
+      <c r="F6">
+        <v>1813</v>
+      </c>
+      <c r="G6">
+        <v>1813</v>
+      </c>
+      <c r="H6">
+        <v>1813</v>
+      </c>
+      <c r="I6">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="14" spans="1:53">
+      <c r="AM14" t="s">
+        <v>19</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:53">
+      <c r="AM15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AN15">
+        <v>1</v>
+      </c>
+      <c r="AO15">
+        <v>2</v>
+      </c>
+      <c r="AP15">
+        <v>4</v>
+      </c>
+      <c r="AQ15">
+        <v>8</v>
+      </c>
+      <c r="AR15">
+        <v>16</v>
+      </c>
+      <c r="AS15">
+        <v>32</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>14</v>
+      </c>
+      <c r="AV15">
+        <v>1</v>
+      </c>
+      <c r="AW15">
+        <v>2</v>
+      </c>
+      <c r="AX15">
+        <v>4</v>
+      </c>
+      <c r="AY15">
+        <v>8</v>
+      </c>
+      <c r="AZ15">
+        <v>16</v>
+      </c>
+      <c r="BA15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:53">
+      <c r="AM16" t="s">
         <v>15</v>
       </c>
-      <c r="N3">
+      <c r="AN16">
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="AO16">
         <v>0.50029999999999997</v>
       </c>
-      <c r="P3">
+      <c r="AP16">
         <v>0.25040000000000001</v>
       </c>
-      <c r="Q3">
+      <c r="AQ16">
         <f>0.1256</f>
         <v>0.12559999999999999</v>
       </c>
-      <c r="R3">
+      <c r="AR16">
         <f>0.0634</f>
         <v>6.3399999999999998E-2</v>
       </c>
-      <c r="S3">
+      <c r="AS16">
         <f>0.0319</f>
         <v>3.1899999999999998E-2</v>
       </c>
-      <c r="U3" t="s">
+      <c r="AU16" t="s">
         <v>15</v>
       </c>
-      <c r="V3">
+      <c r="AV16">
         <v>1</v>
       </c>
-      <c r="W3">
+      <c r="AW16">
         <v>0.50019999999999998</v>
       </c>
-      <c r="X3">
+      <c r="AX16">
         <v>0.25040000000000001</v>
       </c>
-      <c r="Y3">
+      <c r="AY16">
         <v>0.12520000000000001</v>
       </c>
-      <c r="Z3">
+      <c r="AZ16">
         <v>6.3E-2</v>
       </c>
-      <c r="AA3">
+      <c r="BA16">
         <v>3.15E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>1248</v>
-      </c>
-      <c r="C4">
-        <v>642</v>
-      </c>
-      <c r="D4">
-        <v>434</v>
-      </c>
-      <c r="E4">
-        <v>344</v>
-      </c>
-      <c r="F4">
-        <v>315</v>
-      </c>
-      <c r="G4">
-        <v>307</v>
-      </c>
-      <c r="H4">
-        <v>298</v>
-      </c>
-      <c r="I4">
-        <v>298</v>
-      </c>
-      <c r="M4" t="s">
+    <row r="17" spans="39:53">
+      <c r="AM17" t="s">
         <v>16</v>
       </c>
-      <c r="N4">
+      <c r="AN17">
         <v>1</v>
       </c>
-      <c r="O4">
+      <c r="AO17">
         <v>0.50049999999999994</v>
       </c>
-      <c r="P4">
+      <c r="AP17">
         <v>0.25040000000000001</v>
       </c>
-      <c r="Q4">
+      <c r="AQ17">
         <v>0.12559999999999999</v>
       </c>
-      <c r="R4">
+      <c r="AR17">
         <v>6.3399999999999998E-2</v>
       </c>
-      <c r="S4">
+      <c r="AS17">
         <f>0.0319</f>
         <v>3.1899999999999998E-2</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AU17" t="s">
         <v>16</v>
       </c>
-      <c r="V4">
+      <c r="AV17">
         <v>1</v>
       </c>
-      <c r="W4">
+      <c r="AW17">
         <v>0.50060000000000004</v>
       </c>
-      <c r="X4">
+      <c r="AX17">
         <v>0.25080000000000002</v>
       </c>
-      <c r="Y4">
+      <c r="AY17">
         <v>0.1255</v>
       </c>
-      <c r="Z4">
+      <c r="AZ17">
         <v>6.3299999999999995E-2</v>
       </c>
-      <c r="AA4">
+      <c r="BA17">
         <v>3.2099999999999997E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>535</v>
-      </c>
-      <c r="C5">
-        <v>535</v>
-      </c>
-      <c r="D5">
-        <v>535</v>
-      </c>
-      <c r="E5">
-        <v>535</v>
-      </c>
-      <c r="F5">
-        <v>535</v>
-      </c>
-      <c r="G5">
-        <v>535</v>
-      </c>
-      <c r="H5">
-        <v>535</v>
-      </c>
-      <c r="I5">
-        <v>535</v>
-      </c>
-      <c r="M5" t="s">
+    <row r="18" spans="39:53">
+      <c r="AM18" t="s">
         <v>17</v>
       </c>
-      <c r="N5">
+      <c r="AN18">
         <v>1</v>
       </c>
-      <c r="O5">
+      <c r="AO18">
         <v>0.50170000000000003</v>
       </c>
-      <c r="P5">
+      <c r="AP18">
         <v>0.49690000000000001</v>
       </c>
-      <c r="Q5">
+      <c r="AQ18">
         <v>0.44230000000000003</v>
       </c>
-      <c r="R5">
+      <c r="AR18">
         <v>0.42559999999999998</v>
       </c>
-      <c r="S5">
+      <c r="AS18">
         <v>0.42149999999999999</v>
       </c>
-      <c r="U5" t="s">
+      <c r="AU18" t="s">
         <v>17</v>
       </c>
-      <c r="V5">
+      <c r="AV18">
         <v>1</v>
       </c>
-      <c r="W5">
+      <c r="AW18">
         <v>0.50129999999999997</v>
       </c>
-      <c r="X5">
+      <c r="AX18">
         <v>0.34320000000000001</v>
       </c>
-      <c r="Y5">
+      <c r="AY18">
         <v>0.35709999999999997</v>
       </c>
-      <c r="Z5">
+      <c r="AZ18">
         <v>0.32619999999999999</v>
       </c>
-      <c r="AA5">
+      <c r="BA18">
         <v>0.31259999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>1813</v>
-      </c>
-      <c r="C6">
-        <v>1813</v>
-      </c>
-      <c r="D6">
-        <v>1813</v>
-      </c>
-      <c r="E6">
-        <v>1813</v>
-      </c>
-      <c r="F6">
-        <v>1813</v>
-      </c>
-      <c r="G6">
-        <v>1813</v>
-      </c>
-      <c r="H6">
-        <v>1813</v>
-      </c>
-      <c r="I6">
-        <v>1813</v>
-      </c>
-      <c r="M6" t="s">
+    <row r="19" spans="39:53">
+      <c r="AM19" t="s">
         <v>18</v>
       </c>
-      <c r="N6">
+      <c r="AN19">
         <v>1</v>
       </c>
-      <c r="O6">
+      <c r="AO19">
         <v>0.50049999999999994</v>
       </c>
-      <c r="P6">
+      <c r="AP19">
         <v>0.31040000000000001</v>
       </c>
-      <c r="Q6">
+      <c r="AQ19">
         <v>0.13189999999999999</v>
       </c>
-      <c r="R6">
+      <c r="AR19">
         <f>0.1029</f>
         <v>0.10290000000000001</v>
       </c>
-      <c r="S6">
+      <c r="AS19">
         <v>0.1065</v>
       </c>
-      <c r="U6" t="s">
+      <c r="AU19" t="s">
         <v>18</v>
       </c>
-      <c r="V6">
+      <c r="AV19">
         <v>1</v>
       </c>
-      <c r="W6">
+      <c r="AW19">
         <v>0.50029999999999997</v>
       </c>
-      <c r="X6">
+      <c r="AX19">
         <v>0.27950000000000003</v>
       </c>
-      <c r="Y6">
+      <c r="AY19">
         <v>0.18140000000000001</v>
       </c>
-      <c r="Z6">
+      <c r="AZ19">
         <v>0.11840000000000001</v>
       </c>
-      <c r="AA6">
+      <c r="BA19">
         <v>0.1057</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
-      <c r="M9" t="s">
+    <row r="22" spans="39:53">
+      <c r="AM22" t="s">
         <v>21</v>
       </c>
-      <c r="U9" t="s">
+      <c r="AU22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
-      <c r="M10" t="s">
+    <row r="23" spans="39:53">
+      <c r="AM23" t="s">
         <v>14</v>
       </c>
-      <c r="N10">
+      <c r="AN23">
         <v>1</v>
       </c>
-      <c r="O10">
+      <c r="AO23">
         <v>2</v>
       </c>
-      <c r="P10">
+      <c r="AP23">
         <v>4</v>
       </c>
-      <c r="Q10">
+      <c r="AQ23">
         <v>8</v>
       </c>
-      <c r="R10">
+      <c r="AR23">
         <v>16</v>
       </c>
-      <c r="S10">
+      <c r="AS23">
         <v>32</v>
       </c>
-      <c r="U10" t="s">
+      <c r="AU23" t="s">
         <v>14</v>
       </c>
-      <c r="V10">
+      <c r="AV23">
         <v>1</v>
       </c>
-      <c r="W10">
+      <c r="AW23">
         <v>2</v>
       </c>
-      <c r="X10">
+      <c r="AX23">
         <v>4</v>
       </c>
-      <c r="Y10">
+      <c r="AY23">
         <v>8</v>
       </c>
-      <c r="Z10">
+      <c r="AZ23">
         <v>16</v>
       </c>
-      <c r="AA10">
+      <c r="BA23">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
-      <c r="M11" t="s">
+    <row r="24" spans="39:53">
+      <c r="AM24" t="s">
         <v>15</v>
       </c>
-      <c r="N11">
+      <c r="AN24">
         <v>1</v>
       </c>
-      <c r="O11">
+      <c r="AO24">
         <v>0.5</v>
       </c>
-      <c r="P11">
+      <c r="AP24">
         <v>0.25069999999999998</v>
       </c>
-      <c r="Q11">
+      <c r="AQ24">
         <v>0.12540000000000001</v>
       </c>
-      <c r="R11">
+      <c r="AR24">
         <v>6.25E-2</v>
       </c>
-      <c r="S11">
+      <c r="AS24">
         <v>3.1199999999999999E-2</v>
       </c>
-      <c r="U11" t="s">
+      <c r="AU24" t="s">
         <v>15</v>
       </c>
-      <c r="V11">
+      <c r="AV24">
         <v>1</v>
       </c>
-      <c r="W11">
+      <c r="AW24">
         <v>0.49980000000000002</v>
       </c>
-      <c r="X11">
+      <c r="AX24">
         <v>0.24940000000000001</v>
       </c>
-      <c r="Y11">
+      <c r="AY24">
         <v>0.12470000000000001</v>
       </c>
-      <c r="Z11">
+      <c r="AZ24">
         <v>6.1899999999999997E-2</v>
       </c>
-      <c r="AA11">
+      <c r="BA24">
         <v>3.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
-      <c r="M12" t="s">
+    <row r="25" spans="39:53">
+      <c r="AM25" t="s">
         <v>16</v>
       </c>
-      <c r="N12">
+      <c r="AN25">
         <v>1</v>
       </c>
-      <c r="O12">
+      <c r="AO25">
         <v>0.50070000000000003</v>
       </c>
-      <c r="P12">
+      <c r="AP25">
         <v>0.25119999999999998</v>
       </c>
-      <c r="Q12">
+      <c r="AQ25">
         <f>0.1261</f>
         <v>0.12609999999999999</v>
       </c>
-      <c r="R12">
+      <c r="AR25">
         <v>6.3700000000000007E-2</v>
       </c>
-      <c r="S12">
+      <c r="AS25">
         <v>3.2300000000000002E-2</v>
       </c>
-      <c r="U12" t="s">
+      <c r="AU25" t="s">
         <v>16</v>
       </c>
-      <c r="V12">
+      <c r="AV25">
         <v>1</v>
       </c>
-      <c r="W12">
+      <c r="AW25">
         <v>0.501</v>
       </c>
-      <c r="X12">
+      <c r="AX25">
         <v>0.25119999999999998</v>
       </c>
-      <c r="Y12">
+      <c r="AY25">
         <v>0.12690000000000001</v>
       </c>
-      <c r="Z12">
+      <c r="AZ25">
         <v>6.4399999999999999E-2</v>
       </c>
-      <c r="AA12">
+      <c r="BA25">
         <v>3.3000000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:27">
-      <c r="M13" t="s">
+    <row r="26" spans="39:53">
+      <c r="AM26" t="s">
         <v>17</v>
       </c>
-      <c r="N13">
+      <c r="AN26">
         <v>1</v>
       </c>
-      <c r="O13">
+      <c r="AO26">
         <v>0.50170000000000003</v>
       </c>
-      <c r="P13">
+      <c r="AP26">
         <v>0.27400000000000002</v>
       </c>
-      <c r="Q13">
+      <c r="AQ26">
         <v>0.1603</v>
       </c>
-      <c r="R13">
+      <c r="AR26">
         <v>0.14050000000000001</v>
       </c>
-      <c r="S13">
+      <c r="AS26">
         <f>0.1264</f>
         <v>0.12640000000000001</v>
       </c>
-      <c r="U13" t="s">
+      <c r="AU26" t="s">
         <v>17</v>
       </c>
-      <c r="V13">
+      <c r="AV26">
         <v>1</v>
       </c>
-      <c r="W13">
+      <c r="AW26">
         <v>0.5081</v>
       </c>
-      <c r="X13">
+      <c r="AX26">
         <v>0.14940000000000001</v>
       </c>
-      <c r="Y13">
+      <c r="AY26">
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="Z13">
+      <c r="AZ26">
         <v>0</v>
       </c>
-      <c r="AA13">
+      <c r="BA26">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
-      <c r="M14" t="s">
+    <row r="27" spans="39:53">
+      <c r="AM27" t="s">
         <v>18</v>
       </c>
-      <c r="N14">
+      <c r="AN27">
         <v>1</v>
       </c>
-      <c r="O14">
+      <c r="AO27">
         <v>0.50209999999999999</v>
       </c>
-      <c r="P14">
+      <c r="AP27">
         <v>0.28029999999999999</v>
       </c>
-      <c r="Q14">
+      <c r="AQ27">
         <f>0.145</f>
         <v>0.14499999999999999</v>
       </c>
-      <c r="R14">
+      <c r="AR27">
         <v>9.4600000000000004E-2</v>
       </c>
-      <c r="S14">
+      <c r="AS27">
         <v>6.6799999999999998E-2</v>
       </c>
-      <c r="U14" t="s">
+      <c r="AU27" t="s">
         <v>18</v>
       </c>
-      <c r="V14">
+      <c r="AV27">
         <v>1</v>
       </c>
-      <c r="W14">
+      <c r="AW27">
         <v>0.63700000000000001</v>
       </c>
-      <c r="X14">
+      <c r="AX27">
         <v>0.40899999999999997</v>
       </c>
-      <c r="Y14">
+      <c r="AY27">
         <v>0.23710000000000001</v>
       </c>
-      <c r="Z14">
+      <c r="AZ27">
         <v>0.2354</v>
       </c>
-      <c r="AA14">
+      <c r="BA27">
         <v>0.23180000000000001</v>
       </c>
     </row>
-    <row r="25" spans="13:17">
-      <c r="N25" t="s">
+    <row r="38" spans="39:43">
+      <c r="AN38" t="s">
         <v>28</v>
       </c>
-      <c r="O25" t="s">
+      <c r="AO38" t="s">
         <v>27</v>
       </c>
-      <c r="P25" t="s">
+      <c r="AP38" t="s">
         <v>29</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="AQ38" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="13:17">
-      <c r="M26" t="s">
+    <row r="39" spans="39:43">
+      <c r="AM39" t="s">
         <v>23</v>
       </c>
-      <c r="N26">
+      <c r="AN39">
         <v>0.49690000000000001</v>
       </c>
-      <c r="O26">
+      <c r="AO39">
         <v>0.37319999999999998</v>
       </c>
-      <c r="P26">
+      <c r="AP39">
         <v>0.27400000000000002</v>
       </c>
-      <c r="Q26">
+      <c r="AQ39">
         <v>0.14940000000000001</v>
       </c>
     </row>
-    <row r="27" spans="13:17">
-      <c r="M27" t="s">
+    <row r="40" spans="39:43">
+      <c r="AM40" t="s">
         <v>24</v>
       </c>
-      <c r="N27">
+      <c r="AN40">
         <v>0.44230000000000003</v>
       </c>
-      <c r="O27">
+      <c r="AO40">
         <v>0.35709999999999997</v>
       </c>
-      <c r="P27">
+      <c r="AP40">
         <v>0.1603</v>
       </c>
-      <c r="Q27">
+      <c r="AQ40">
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="28" spans="13:17">
-      <c r="M28" t="s">
+    <row r="41" spans="39:43">
+      <c r="AM41" t="s">
         <v>25</v>
       </c>
-      <c r="N28">
+      <c r="AN41">
         <v>0.42559999999999998</v>
       </c>
-      <c r="O28">
+      <c r="AO41">
         <v>0.32619999999999999</v>
       </c>
-      <c r="P28">
+      <c r="AP41">
         <v>0.14050000000000001</v>
       </c>
-      <c r="Q28">
+      <c r="AQ41">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="13:17">
-      <c r="M29" t="s">
+    <row r="42" spans="39:43">
+      <c r="AM42" t="s">
         <v>26</v>
       </c>
-      <c r="N29">
+      <c r="AN42">
         <v>0.42149999999999999</v>
       </c>
-      <c r="O29">
+      <c r="AO42">
         <v>0.31259999999999999</v>
       </c>
-      <c r="P29">
+      <c r="AP42">
         <v>0.12640000000000001</v>
       </c>
-      <c r="Q29">
+      <c r="AQ42">
         <v>0</v>
       </c>
     </row>
@@ -15338,13 +15551,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6E50E1-FA69-4847-B614-76E5EFFC3D26}">
-  <dimension ref="A2:AD26"/>
+  <dimension ref="A2:AD59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:30">
       <c r="P2" t="s">
@@ -15427,25 +15644,25 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>8920</v>
+        <v>6648</v>
       </c>
       <c r="C4">
-        <v>6004</v>
+        <v>3908</v>
       </c>
       <c r="D4">
-        <v>4458</v>
+        <v>2437</v>
       </c>
       <c r="E4">
-        <v>3746</v>
+        <v>1766</v>
       </c>
       <c r="F4">
-        <v>3332</v>
+        <v>1547</v>
       </c>
       <c r="G4">
-        <v>3111</v>
+        <v>1421</v>
       </c>
       <c r="H4">
-        <v>2915</v>
+        <v>1358</v>
       </c>
       <c r="P4" t="s">
         <v>15</v>
@@ -15498,25 +15715,25 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>7419</v>
+        <v>6327</v>
       </c>
       <c r="C5">
-        <v>5618</v>
+        <v>3649</v>
       </c>
       <c r="D5">
-        <v>4219</v>
+        <v>2187</v>
       </c>
       <c r="E5">
-        <v>3639</v>
+        <v>1799</v>
       </c>
       <c r="F5">
-        <v>3198</v>
+        <v>1643</v>
       </c>
       <c r="G5">
-        <v>3008</v>
+        <v>1504</v>
       </c>
       <c r="H5">
-        <v>3010</v>
+        <v>1517</v>
       </c>
       <c r="P5" t="s">
         <v>16</v>
@@ -15567,25 +15784,25 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>2141</v>
+        <v>2868</v>
       </c>
       <c r="C6">
-        <v>2141</v>
+        <v>2868</v>
       </c>
       <c r="D6">
-        <v>2141</v>
+        <v>2868</v>
       </c>
       <c r="E6">
-        <v>2141</v>
+        <v>2868</v>
       </c>
       <c r="F6">
-        <v>2141</v>
+        <v>2868</v>
       </c>
       <c r="G6">
-        <v>2141</v>
+        <v>2868</v>
       </c>
       <c r="H6">
-        <v>2141</v>
+        <v>2868</v>
       </c>
       <c r="P6" t="s">
         <v>17</v>
@@ -15632,28 +15849,28 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B7">
-        <v>6283</v>
+        <v>2141</v>
       </c>
       <c r="C7">
-        <v>6283</v>
+        <v>2141</v>
       </c>
       <c r="D7">
-        <v>6283</v>
+        <v>2141</v>
       </c>
       <c r="E7">
-        <v>6283</v>
+        <v>2141</v>
       </c>
       <c r="F7">
-        <v>6283</v>
+        <v>2141</v>
       </c>
       <c r="G7">
-        <v>6283</v>
+        <v>2141</v>
       </c>
       <c r="H7">
-        <v>6283</v>
+        <v>2141</v>
       </c>
       <c r="P7" t="s">
         <v>18</v>
@@ -15697,6 +15914,32 @@
       </c>
       <c r="AD7">
         <v>0.1057</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>6283</v>
+      </c>
+      <c r="C8">
+        <v>6283</v>
+      </c>
+      <c r="D8">
+        <v>6283</v>
+      </c>
+      <c r="E8">
+        <v>6283</v>
+      </c>
+      <c r="F8">
+        <v>6283</v>
+      </c>
+      <c r="G8">
+        <v>6283</v>
+      </c>
+      <c r="H8">
+        <v>6283</v>
       </c>
     </row>
     <row r="10" spans="1:30">
@@ -16012,7 +16255,121 @@
         <v>0</v>
       </c>
     </row>
+    <row r="49" spans="1:4">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C50">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="4"/>
+      <c r="B51" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1009</v>
+      </c>
+      <c r="D51">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="4"/>
+      <c r="B53" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="5"/>
+      <c r="B55" t="s">
+        <v>39</v>
+      </c>
+      <c r="C55">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="5"/>
+      <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="5"/>
+      <c r="B57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="3">
+        <v>661</v>
+      </c>
+      <c r="D57">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="B58" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58">
+        <v>2539</v>
+      </c>
+      <c r="D58">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="B59" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59">
+        <v>2815</v>
+      </c>
+      <c r="D59">
+        <v>1358</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A50:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A54:A57"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>